<commit_message>
Update to latest 4.0 files
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CC6B04-B346-4890-A318-734C137A4431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A8C306-3056-445E-B8CA-ED2622C8BF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="22875" windowHeight="23115" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -842,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.46666666699999998</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>